<commit_message>
add zssessential and zssdemo3
</commit_message>
<xml_diff>
--- a/essential/src/main/webapp/WEB-INF/excelsrc/copyPasteBase.xlsx
+++ b/essential/src/main/webapp/WEB-INF/excelsrc/copyPasteBase.xlsx
@@ -4,22 +4,33 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18240" windowHeight="11280" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="17460" windowHeight="9465" tabRatio="781" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Protected (1111)" sheetId="2" r:id="rId2"/>
-    <sheet name="UnProtected" sheetId="3" r:id="rId3"/>
-    <sheet name="merge&amp;unMerge" sheetId="4" r:id="rId4"/>
-    <sheet name="AutoFilter" sheetId="5" r:id="rId5"/>
-    <sheet name="Chart" sheetId="6" r:id="rId6"/>
+    <sheet name="HyperLink" sheetId="14" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Protected (1111)" sheetId="2" r:id="rId3"/>
+    <sheet name="UnProtected" sheetId="3" r:id="rId4"/>
+    <sheet name="merge&amp;unMerge" sheetId="4" r:id="rId5"/>
+    <sheet name="AutoFilter" sheetId="5" r:id="rId6"/>
+    <sheet name="AutoFilter Off" sheetId="8" r:id="rId7"/>
+    <sheet name="Chart" sheetId="6" r:id="rId8"/>
+    <sheet name="Chart Inside" sheetId="13" r:id="rId9"/>
+    <sheet name="CellValue" sheetId="7" r:id="rId10"/>
+    <sheet name="Image" sheetId="12" r:id="rId11"/>
+    <sheet name="AutoFill" sheetId="9" r:id="rId12"/>
+    <sheet name="Validation" sheetId="10" r:id="rId13"/>
+    <sheet name="Validation NPE" sheetId="11" r:id="rId14"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">AutoFilter!$C$4:$E$11</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>ABC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -198,6 +209,96 @@
   </si>
   <si>
     <t>SUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dennis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String drop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;-Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number direct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date direct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String (empty ref)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B3:J22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zkoss http</t>
+  </si>
+  <si>
+    <t>Mail dennis</t>
+  </si>
+  <si>
+    <t>AAAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBBBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>toggle merge center here (long long long long text)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,10 +306,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +364,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -434,12 +552,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -498,6 +620,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -510,16 +650,974 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>843</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>772</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>926</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1352</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1982</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="42889216"/>
+        <c:axId val="42890752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="42889216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42890752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42890752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42889216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>843</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>772</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart Inside'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Chart Inside'!$B$3:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart Inside'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>926</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1352</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1982</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="42925056"/>
+        <c:axId val="41632512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="42925056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41632512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="41632512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42925056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Sunset.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="876300" y="552450"/>
+          <a:ext cx="4902200" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -807,9 +1905,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="43.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="32.25">
+      <c r="B8" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="e">
+        <f ca="1">XYZ()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="20">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <f>SUM(B1:B3)</f>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <f>SUM(C1:C3)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>SUM(D1:D3)</f>
+        <v>123655.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="21">
+        <v>41275</v>
+      </c>
+      <c r="J3" s="21">
+        <v>41275</v>
+      </c>
+      <c r="K3" s="21">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21">
+        <v>41276</v>
+      </c>
+      <c r="K4" s="21">
+        <v>41306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="21">
+        <v>41277</v>
+      </c>
+      <c r="K5" s="21">
+        <v>41334</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11">
+      <c r="B3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="22">
+        <v>41275</v>
+      </c>
+      <c r="I7" s="22">
+        <v>41305</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>$H$5:$K$5</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>H3</formula1>
+      <formula2>I3</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+      <formula1>41275</formula1>
+      <formula2>41639</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+      <formula1>H7</formula1>
+      <formula2>I7</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+      <formula1>41275</formula1>
+      <formula2>41305</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9">
+      <c r="B3" s="21"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="21"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="C8" s="22"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+      <formula1>$H$6:$K$6</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -902,7 +2386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:E7"/>
   <sheetViews>
@@ -940,7 +2424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:C4"/>
   <sheetViews>
@@ -966,12 +2450,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D4:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -981,10 +2465,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:9">
-      <c r="D4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="20"/>
+      <c r="D4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="26"/>
       <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
@@ -992,17 +2476,17 @@
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="4:9">
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="G5" s="13"/>
       <c r="H5" s="16"/>
       <c r="I5" s="14"/>
     </row>
     <row r="7" spans="4:9">
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="26"/>
       <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
@@ -1010,8 +2494,8 @@
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="4:9">
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
       <c r="G8" s="13"/>
       <c r="H8" s="16"/>
       <c r="I8" s="14"/>
@@ -1040,7 +2524,115 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="C4:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="4" spans="3:5">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" hidden="1">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" hidden="1">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" hidden="1">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C4:E11">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Day1"/>
+        <filter val="Day4"/>
+        <filter val="Day5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:E11"/>
   <sheetViews>
@@ -1138,32 +2730,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C3">
@@ -1181,7 +2773,7 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C4">
@@ -1199,7 +2791,7 @@
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C5">
@@ -1217,7 +2809,7 @@
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C6">
@@ -1235,7 +2827,7 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C7">
@@ -1253,7 +2845,7 @@
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>35</v>
       </c>
       <c r="C8">
@@ -1271,7 +2863,7 @@
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="19" t="s">
         <v>36</v>
       </c>
       <c r="C9">
@@ -1289,7 +2881,7 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C10">
@@ -1307,7 +2899,7 @@
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C11">
@@ -1325,7 +2917,7 @@
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="19" t="s">
         <v>39</v>
       </c>
       <c r="C12">
@@ -1346,4 +2938,215 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="C2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>875</v>
+      </c>
+      <c r="F3">
+        <f>SUM(C3:E3)</f>
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>554</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F12" si="0">SUM(C4:E4)</f>
+        <v>798</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>283</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>843</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>102</v>
+      </c>
+      <c r="E7">
+        <v>324</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>926</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
+      </c>
+      <c r="D8">
+        <v>276</v>
+      </c>
+      <c r="E8">
+        <v>476</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="D9">
+        <v>432</v>
+      </c>
+      <c r="E9">
+        <v>123</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>800</v>
+      </c>
+      <c r="D10">
+        <v>572</v>
+      </c>
+      <c r="E10">
+        <v>351</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>900</v>
+      </c>
+      <c r="D11">
+        <v>432</v>
+      </c>
+      <c r="E11">
+        <v>672</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>210</v>
+      </c>
+      <c r="E12">
+        <v>772</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1982</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>